<commit_message>
#CRM-177 District Field in SF list Excel
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/SF_List_Template.xlsx
+++ b/application/controllers/excel-templates/SF_List_Template.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around-aws\application\controllers\excel-templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around\application\controllers\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
   <si>
     <t>Pincode</t>
   </si>
@@ -216,12 +216,15 @@
   </si>
   <si>
     <t>ID</t>
+  </si>
+  <si>
+    <t>District</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -554,11 +557,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AH2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AI2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -575,29 +578,29 @@
     <col min="10" max="10" width="17.7109375" customWidth="1"/>
     <col min="11" max="11" width="17.28515625" customWidth="1"/>
     <col min="12" max="12" width="26.85546875" customWidth="1"/>
-    <col min="13" max="13" width="37.5703125" customWidth="1"/>
-    <col min="14" max="14" width="28" customWidth="1"/>
-    <col min="15" max="15" width="23.42578125" customWidth="1"/>
-    <col min="16" max="16" width="25.5703125" customWidth="1"/>
-    <col min="17" max="17" width="15.5703125" customWidth="1"/>
-    <col min="18" max="18" width="24.5703125" customWidth="1"/>
-    <col min="19" max="19" width="22.28515625" customWidth="1"/>
-    <col min="20" max="20" width="20.42578125" customWidth="1"/>
-    <col min="21" max="21" width="22" customWidth="1"/>
-    <col min="22" max="22" width="25.140625" customWidth="1"/>
-    <col min="23" max="23" width="23.42578125" customWidth="1"/>
-    <col min="24" max="24" width="25.5703125" customWidth="1"/>
-    <col min="25" max="25" width="25.28515625" customWidth="1"/>
-    <col min="26" max="26" width="27" customWidth="1"/>
-    <col min="27" max="27" width="31.85546875" customWidth="1"/>
-    <col min="28" max="28" width="29.140625" customWidth="1"/>
-    <col min="29" max="29" width="30.42578125" customWidth="1"/>
-    <col min="30" max="30" width="27.140625" customWidth="1"/>
-    <col min="31" max="31" width="30.140625" customWidth="1"/>
-    <col min="32" max="34" width="21.140625" customWidth="1"/>
+    <col min="13" max="14" width="37.5703125" customWidth="1"/>
+    <col min="15" max="15" width="28" customWidth="1"/>
+    <col min="16" max="16" width="23.42578125" customWidth="1"/>
+    <col min="17" max="17" width="25.5703125" customWidth="1"/>
+    <col min="18" max="18" width="15.5703125" customWidth="1"/>
+    <col min="19" max="19" width="24.5703125" customWidth="1"/>
+    <col min="20" max="20" width="22.28515625" customWidth="1"/>
+    <col min="21" max="21" width="20.42578125" customWidth="1"/>
+    <col min="22" max="22" width="22" customWidth="1"/>
+    <col min="23" max="23" width="25.140625" customWidth="1"/>
+    <col min="24" max="24" width="23.42578125" customWidth="1"/>
+    <col min="25" max="25" width="25.5703125" customWidth="1"/>
+    <col min="26" max="26" width="25.28515625" customWidth="1"/>
+    <col min="27" max="27" width="27" customWidth="1"/>
+    <col min="28" max="28" width="31.85546875" customWidth="1"/>
+    <col min="29" max="29" width="29.140625" customWidth="1"/>
+    <col min="30" max="30" width="30.42578125" customWidth="1"/>
+    <col min="31" max="31" width="27.140625" customWidth="1"/>
+    <col min="32" max="32" width="30.140625" customWidth="1"/>
+    <col min="33" max="35" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -638,66 +641,69 @@
         <v>22</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>57</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="AG1" s="1"/>
       <c r="AH1" s="1"/>
+      <c r="AI1" s="1"/>
     </row>
-    <row r="2" spans="1:34" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -738,60 +744,63 @@
         <v>23</v>
       </c>
       <c r="N2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="O2" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>46</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AA2" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="AA2" s="6" t="s">
+      <c r="AB2" s="6" t="s">
         <v>50</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AD2" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="AD2" s="3" t="s">
+      <c r="AE2" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="AE2" s="3" t="s">
+      <c r="AF2" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="AF2" s="3" t="s">
+      <c r="AG2" s="3" t="s">
         <v>60</v>
       </c>
     </row>

</xml_diff>

<commit_message>
#CRM-31 Remove ID, Bank Details, bracket flag from Download SF list
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/SF_List_Template.xlsx
+++ b/application/controllers/excel-templates/SF_List_Template.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19001"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
   <si>
     <t>Pincode</t>
   </si>
@@ -41,9 +41,6 @@
     <t>{vendor:name}</t>
   </si>
   <si>
-    <t>{vendor:id}</t>
-  </si>
-  <si>
     <t>Address</t>
   </si>
   <si>
@@ -167,30 +164,6 @@
     <t>{vendor:create_date}</t>
   </si>
   <si>
-    <t>Bank Name</t>
-  </si>
-  <si>
-    <t>{vendor:bank_name}</t>
-  </si>
-  <si>
-    <t>Bank Account</t>
-  </si>
-  <si>
-    <t>{vendor:bank_account}</t>
-  </si>
-  <si>
-    <t>IFSC Code</t>
-  </si>
-  <si>
-    <t>{vendor:ifsc_code}</t>
-  </si>
-  <si>
-    <t>Beneficiary Name</t>
-  </si>
-  <si>
-    <t>{vendor:beneficiary_name}</t>
-  </si>
-  <si>
     <t>Non-working Day</t>
   </si>
   <si>
@@ -203,19 +176,10 @@
     <t>{vendor:sc_code}</t>
   </si>
   <si>
-    <t>Brackets Flag</t>
-  </si>
-  <si>
-    <t>{vendor:brackets_flag}</t>
-  </si>
-  <si>
     <t>{vendor:primary_contact_email}</t>
   </si>
   <si>
     <t>{vendor:phone_2}</t>
-  </si>
-  <si>
-    <t>ID</t>
   </si>
   <si>
     <t>District</t>
@@ -262,7 +226,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -275,9 +239,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -558,157 +519,134 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AI2"/>
+  <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AA13" sqref="AA13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="37.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" customWidth="1"/>
-    <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="5" width="24.140625" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="24.5703125" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" customWidth="1"/>
-    <col min="12" max="12" width="26.85546875" customWidth="1"/>
-    <col min="13" max="14" width="37.5703125" customWidth="1"/>
-    <col min="15" max="15" width="28" customWidth="1"/>
-    <col min="16" max="16" width="23.42578125" customWidth="1"/>
-    <col min="17" max="17" width="25.5703125" customWidth="1"/>
-    <col min="18" max="18" width="15.5703125" customWidth="1"/>
-    <col min="19" max="19" width="24.5703125" customWidth="1"/>
-    <col min="20" max="20" width="22.28515625" customWidth="1"/>
-    <col min="21" max="21" width="20.42578125" customWidth="1"/>
-    <col min="22" max="22" width="22" customWidth="1"/>
-    <col min="23" max="23" width="25.140625" customWidth="1"/>
-    <col min="24" max="24" width="23.42578125" customWidth="1"/>
-    <col min="25" max="25" width="25.5703125" customWidth="1"/>
-    <col min="26" max="26" width="25.28515625" customWidth="1"/>
-    <col min="27" max="27" width="27" customWidth="1"/>
-    <col min="28" max="28" width="31.85546875" customWidth="1"/>
-    <col min="29" max="29" width="29.140625" customWidth="1"/>
-    <col min="30" max="30" width="30.42578125" customWidth="1"/>
-    <col min="31" max="31" width="27.140625" customWidth="1"/>
-    <col min="32" max="32" width="30.140625" customWidth="1"/>
-    <col min="33" max="35" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" customWidth="1"/>
+    <col min="5" max="5" width="19.85546875" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
+    <col min="7" max="7" width="24.5703125" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" customWidth="1"/>
+    <col min="9" max="9" width="17.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.28515625" customWidth="1"/>
+    <col min="11" max="11" width="26.85546875" customWidth="1"/>
+    <col min="12" max="13" width="37.5703125" customWidth="1"/>
+    <col min="14" max="14" width="28" customWidth="1"/>
+    <col min="15" max="15" width="23.42578125" customWidth="1"/>
+    <col min="16" max="16" width="25.5703125" customWidth="1"/>
+    <col min="17" max="17" width="15.5703125" customWidth="1"/>
+    <col min="18" max="18" width="24.5703125" customWidth="1"/>
+    <col min="19" max="19" width="22.28515625" customWidth="1"/>
+    <col min="20" max="20" width="20.42578125" customWidth="1"/>
+    <col min="21" max="21" width="22" customWidth="1"/>
+    <col min="22" max="22" width="25.140625" customWidth="1"/>
+    <col min="23" max="23" width="23.42578125" customWidth="1"/>
+    <col min="24" max="24" width="25.5703125" customWidth="1"/>
+    <col min="25" max="25" width="25.28515625" customWidth="1"/>
+    <col min="26" max="26" width="27.140625" customWidth="1"/>
+    <col min="27" max="27" width="30.140625" customWidth="1"/>
+    <col min="28" max="29" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>63</v>
+        <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>0</v>
       </c>
+      <c r="F1" s="2" t="s">
+        <v>10</v>
+      </c>
       <c r="G1" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="K1" s="2" t="s">
         <v>19</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>22</v>
+        <v>52</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>64</v>
+        <v>23</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="V1" s="2" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="W1" s="2" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="X1" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="Y1" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="Z1" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="AA1" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB1" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC1" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AD1" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE1" s="2" t="s">
-        <v>55</v>
-      </c>
-      <c r="AF1" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="AH1" s="1"/>
-      <c r="AI1" s="1"/>
+        <v>48</v>
+      </c>
+      <c r="AB1" s="1"/>
+      <c r="AC1" s="1"/>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>7</v>
@@ -720,88 +658,70 @@
         <v>9</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="5" t="s">
-        <v>62</v>
+        <v>17</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="K2" s="3" t="s">
+        <v>20</v>
       </c>
       <c r="L2" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>23</v>
+        <v>7</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>8</v>
+        <v>24</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="R2" s="3" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="T2" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="U2" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="V2" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="W2" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="X2" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>46</v>
+        <v>43</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>45</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>47</v>
       </c>
       <c r="AA2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="AB2" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="AC2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="AD2" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="AF2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="AG2" s="3" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Covered states by sf in sf download list
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/SF_List_Template.xlsx
+++ b/application/controllers/excel-templates/SF_List_Template.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>Pincode</t>
   </si>
@@ -183,6 +183,12 @@
   </si>
   <si>
     <t>District</t>
+  </si>
+  <si>
+    <t>Covered_States</t>
+  </si>
+  <si>
+    <t>{vendor:covered_state}</t>
   </si>
 </sst>
 </file>
@@ -519,10 +525,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AC2"/>
+  <dimension ref="A1:AD2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
-      <selection activeCell="AA13" sqref="AA13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -530,33 +536,33 @@
     <col min="1" max="1" width="37.42578125" customWidth="1"/>
     <col min="2" max="2" width="36.7109375" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" customWidth="1"/>
-    <col min="5" max="5" width="19.85546875" customWidth="1"/>
-    <col min="6" max="6" width="18" customWidth="1"/>
-    <col min="7" max="7" width="24.5703125" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
-    <col min="10" max="10" width="17.28515625" customWidth="1"/>
-    <col min="11" max="11" width="26.85546875" customWidth="1"/>
-    <col min="12" max="13" width="37.5703125" customWidth="1"/>
-    <col min="14" max="14" width="28" customWidth="1"/>
-    <col min="15" max="15" width="23.42578125" customWidth="1"/>
-    <col min="16" max="16" width="25.5703125" customWidth="1"/>
-    <col min="17" max="17" width="15.5703125" customWidth="1"/>
-    <col min="18" max="18" width="24.5703125" customWidth="1"/>
-    <col min="19" max="19" width="22.28515625" customWidth="1"/>
-    <col min="20" max="20" width="20.42578125" customWidth="1"/>
-    <col min="21" max="21" width="22" customWidth="1"/>
-    <col min="22" max="22" width="25.140625" customWidth="1"/>
-    <col min="23" max="23" width="23.42578125" customWidth="1"/>
-    <col min="24" max="24" width="25.5703125" customWidth="1"/>
-    <col min="25" max="25" width="25.28515625" customWidth="1"/>
-    <col min="26" max="26" width="27.140625" customWidth="1"/>
-    <col min="27" max="27" width="30.140625" customWidth="1"/>
-    <col min="28" max="29" width="21.140625" customWidth="1"/>
+    <col min="4" max="5" width="24.140625" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="24.5703125" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" customWidth="1"/>
+    <col min="12" max="12" width="26.85546875" customWidth="1"/>
+    <col min="13" max="14" width="37.5703125" customWidth="1"/>
+    <col min="15" max="15" width="28" customWidth="1"/>
+    <col min="16" max="16" width="23.42578125" customWidth="1"/>
+    <col min="17" max="17" width="25.5703125" customWidth="1"/>
+    <col min="18" max="18" width="15.5703125" customWidth="1"/>
+    <col min="19" max="19" width="24.5703125" customWidth="1"/>
+    <col min="20" max="20" width="22.28515625" customWidth="1"/>
+    <col min="21" max="21" width="20.42578125" customWidth="1"/>
+    <col min="22" max="22" width="22" customWidth="1"/>
+    <col min="23" max="23" width="25.140625" customWidth="1"/>
+    <col min="24" max="24" width="23.42578125" customWidth="1"/>
+    <col min="25" max="25" width="25.5703125" customWidth="1"/>
+    <col min="26" max="26" width="25.28515625" customWidth="1"/>
+    <col min="27" max="27" width="27.140625" customWidth="1"/>
+    <col min="28" max="28" width="30.140625" customWidth="1"/>
+    <col min="29" max="30" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
@@ -569,79 +575,82 @@
       <c r="D1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="F1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="AB1" s="1"/>
       <c r="AC1" s="1"/>
+      <c r="AD1" s="1"/>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -655,76 +664,80 @@
         <v>8</v>
       </c>
       <c r="E2" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="J2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>45</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AA2" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>49</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CRM-1637 Show GST number, status and type in download sf list
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/SF_List_Template.xlsx
+++ b/application/controllers/excel-templates/SF_List_Template.xlsx
@@ -1,17 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <workbookPr defaultThemeVersion="166925"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around-adminp-aws\application\controllers\excel-templates\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F268E5B-26D8-4C18-9990-296B35E95921}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
   <sheets>
-    <sheet state="visible" name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Name</t>
   </si>
@@ -173,21 +182,39 @@
   </si>
   <si>
     <t>{vendor:sc_code}</t>
+  </si>
+  <si>
+    <t>GST Number</t>
+  </si>
+  <si>
+    <t>{vendor:gst_no}</t>
+  </si>
+  <si>
+    <t>GST Type</t>
+  </si>
+  <si>
+    <t>{vendor:gst_taxpayer_type}</t>
+  </si>
+  <si>
+    <t>GST Status</t>
+  </si>
+  <si>
+    <t>{vendor:gst_status}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
     <font>
       <b/>
-      <sz val="11.0"/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -197,82 +224,389 @@
       <patternFill patternType="none"/>
     </fill>
     <fill>
-      <patternFill patternType="lightGray"/>
+      <patternFill patternType="gray125"/>
     </fill>
   </fills>
   <borders count="1">
-    <border/>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="center" readingOrder="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" name="Normal" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="44546A"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E7E6E6"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4472C4"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="ED7D31"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="A5A5A5"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="FFC000"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="5B9BD5"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="70AD47"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0563C1"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="954F72"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AF2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="O6" sqref="O6"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="37.43"/>
-    <col customWidth="1" min="2" max="2" width="36.71"/>
-    <col customWidth="1" min="3" max="3" width="22.0"/>
-    <col customWidth="1" min="4" max="5" width="24.14"/>
-    <col customWidth="1" min="6" max="6" width="19.86"/>
-    <col customWidth="1" min="7" max="7" width="18.0"/>
-    <col customWidth="1" min="8" max="8" width="24.57"/>
-    <col customWidth="1" min="9" max="9" width="18.71"/>
-    <col customWidth="1" min="10" max="10" width="17.71"/>
-    <col customWidth="1" min="11" max="11" width="17.29"/>
-    <col customWidth="1" min="12" max="12" width="26.86"/>
-    <col customWidth="1" min="13" max="13" width="37.57"/>
-    <col customWidth="1" min="14" max="14" width="28.0"/>
-    <col customWidth="1" min="15" max="15" width="23.43"/>
-    <col customWidth="1" min="16" max="16" width="25.57"/>
-    <col customWidth="1" min="17" max="17" width="15.57"/>
-    <col customWidth="1" min="18" max="18" width="24.57"/>
-    <col customWidth="1" min="19" max="19" width="22.29"/>
-    <col customWidth="1" min="20" max="20" width="20.43"/>
-    <col customWidth="1" min="21" max="21" width="22.0"/>
-    <col customWidth="1" min="22" max="22" width="25.14"/>
-    <col customWidth="1" min="23" max="23" width="23.43"/>
-    <col customWidth="1" min="24" max="24" width="25.57"/>
-    <col customWidth="1" min="25" max="25" width="25.29"/>
-    <col customWidth="1" min="26" max="26" width="27.14"/>
-    <col customWidth="1" min="27" max="27" width="30.14"/>
-    <col customWidth="1" min="28" max="29" width="21.14"/>
+    <col min="1" max="1" width="37.44140625" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="5" width="24.109375" customWidth="1"/>
+    <col min="6" max="6" width="19.88671875" customWidth="1"/>
+    <col min="7" max="7" width="18" customWidth="1"/>
+    <col min="8" max="8" width="24.5546875" customWidth="1"/>
+    <col min="9" max="9" width="18.6640625" customWidth="1"/>
+    <col min="10" max="10" width="17.6640625" customWidth="1"/>
+    <col min="11" max="11" width="17.33203125" customWidth="1"/>
+    <col min="12" max="15" width="26.88671875" customWidth="1"/>
+    <col min="16" max="16" width="37.5546875" customWidth="1"/>
+    <col min="17" max="17" width="28" customWidth="1"/>
+    <col min="18" max="18" width="23.44140625" customWidth="1"/>
+    <col min="19" max="19" width="25.5546875" customWidth="1"/>
+    <col min="20" max="20" width="15.5546875" customWidth="1"/>
+    <col min="21" max="21" width="24.5546875" customWidth="1"/>
+    <col min="22" max="22" width="22.33203125" customWidth="1"/>
+    <col min="23" max="23" width="20.44140625" customWidth="1"/>
+    <col min="24" max="24" width="22" customWidth="1"/>
+    <col min="25" max="25" width="25.109375" customWidth="1"/>
+    <col min="26" max="26" width="23.44140625" customWidth="1"/>
+    <col min="27" max="27" width="25.5546875" customWidth="1"/>
+    <col min="28" max="28" width="25.33203125" customWidth="1"/>
+    <col min="29" max="29" width="27.109375" customWidth="1"/>
+    <col min="30" max="30" width="30.109375" customWidth="1"/>
+    <col min="31" max="32" width="21.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -309,55 +643,64 @@
       <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="N1" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="O1" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="P1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="AB1" s="4"/>
-      <c r="AC1" s="4"/>
+      <c r="AE1" s="4"/>
+      <c r="AF1" s="4"/>
     </row>
-    <row r="2">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>27</v>
       </c>
@@ -395,52 +738,62 @@
         <v>38</v>
       </c>
       <c r="M2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="P2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="T2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="U2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="V2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="W2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="X2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="Y2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="Z2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="AA2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="AB2" t="s">
         <v>51</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="AC2" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AD2" s="5" t="s">
         <v>53</v>
       </c>
     </row>
   </sheetData>
-  <drawing r:id="rId1"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
CRM 3586 Removed CP from download SF list excel and remove column Service Tax
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/SF_List_Template.xlsx
+++ b/application/controllers/excel-templates/SF_List_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\247around-adminp-aws\application\controllers\excel-templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\XAMPP\htdocs\247_dev\application\controllers\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5214FE20-94EC-4D46-9D8C-8C48C9D292F6}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB5D775-20E5-4992-A0B6-6C3C03DC0B19}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
   <si>
     <t>Name</t>
   </si>
@@ -64,9 +64,6 @@
     <t>Brands</t>
   </si>
   <si>
-    <t>Service Tax No.</t>
-  </si>
-  <si>
     <t>Remarks</t>
   </si>
   <si>
@@ -143,9 +140,6 @@
   </si>
   <si>
     <t>{vendor:brands}</t>
-  </si>
-  <si>
-    <t>{vendor:service_tax_no}</t>
   </si>
   <si>
     <t>{vendor:remarks}</t>
@@ -229,6 +223,7 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -581,45 +576,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AF2"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A1:AE2"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AD11" sqref="AD11"/>
+      <selection activeCell="AF1" sqref="AF1:AF1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="37.44140625" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" customWidth="1"/>
+    <col min="1" max="1" width="37.42578125" customWidth="1"/>
+    <col min="2" max="2" width="36.7109375" customWidth="1"/>
     <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="5" width="24.109375" customWidth="1"/>
-    <col min="6" max="6" width="19.88671875" customWidth="1"/>
+    <col min="4" max="5" width="24.140625" customWidth="1"/>
+    <col min="6" max="6" width="19.85546875" customWidth="1"/>
     <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="24.5546875" customWidth="1"/>
-    <col min="9" max="9" width="18.6640625" customWidth="1"/>
-    <col min="10" max="10" width="17.6640625" customWidth="1"/>
-    <col min="11" max="11" width="17.33203125" customWidth="1"/>
-    <col min="12" max="15" width="26.88671875" customWidth="1"/>
-    <col min="16" max="16" width="37.5546875" customWidth="1"/>
+    <col min="8" max="8" width="24.5703125" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" customWidth="1"/>
+    <col min="10" max="10" width="17.7109375" customWidth="1"/>
+    <col min="11" max="11" width="17.28515625" customWidth="1"/>
+    <col min="12" max="15" width="26.85546875" customWidth="1"/>
+    <col min="16" max="16" width="37.5703125" customWidth="1"/>
     <col min="17" max="17" width="28" customWidth="1"/>
-    <col min="18" max="18" width="23.44140625" customWidth="1"/>
-    <col min="19" max="19" width="25.5546875" customWidth="1"/>
-    <col min="20" max="20" width="15.5546875" customWidth="1"/>
-    <col min="21" max="21" width="24.5546875" customWidth="1"/>
-    <col min="22" max="22" width="22.33203125" customWidth="1"/>
-    <col min="23" max="23" width="20.44140625" customWidth="1"/>
-    <col min="24" max="24" width="22" customWidth="1"/>
-    <col min="25" max="25" width="25.109375" customWidth="1"/>
-    <col min="26" max="26" width="23.44140625" customWidth="1"/>
-    <col min="27" max="27" width="25.5546875" customWidth="1"/>
-    <col min="28" max="28" width="25.33203125" customWidth="1"/>
-    <col min="29" max="29" width="27.109375" customWidth="1"/>
-    <col min="30" max="30" width="30.109375" customWidth="1"/>
-    <col min="31" max="31" width="22.77734375" customWidth="1"/>
-    <col min="32" max="32" width="27.21875" customWidth="1"/>
+    <col min="18" max="18" width="25.5703125" customWidth="1"/>
+    <col min="19" max="19" width="15.5703125" customWidth="1"/>
+    <col min="20" max="20" width="24.5703125" customWidth="1"/>
+    <col min="21" max="21" width="22.28515625" customWidth="1"/>
+    <col min="22" max="22" width="20.42578125" customWidth="1"/>
+    <col min="23" max="23" width="22" customWidth="1"/>
+    <col min="24" max="24" width="25.140625" customWidth="1"/>
+    <col min="25" max="25" width="23.42578125" customWidth="1"/>
+    <col min="26" max="26" width="25.5703125" customWidth="1"/>
+    <col min="27" max="27" width="25.28515625" customWidth="1"/>
+    <col min="28" max="28" width="27.140625" customWidth="1"/>
+    <col min="29" max="29" width="30.140625" customWidth="1"/>
+    <col min="30" max="30" width="22.7109375" customWidth="1"/>
+    <col min="31" max="31" width="27.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -657,13 +652,13 @@
         <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="N1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="O1" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>12</v>
@@ -707,112 +702,106 @@
       <c r="AC1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AD1" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="AE1" s="4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="B2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="K2" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L2" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="M2" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="N2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="O2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="P2" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="Q2" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="R2" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="S2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="T2" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="U2" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="V2" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="W2" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="X2" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y2" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z2" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>49</v>
+      </c>
+      <c r="AB2" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="AC2" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="AD2" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AE2" s="5" t="s">
         <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B2" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="L2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="M2" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="N2" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="O2" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="P2" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="Q2" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="R2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="S2" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="T2" s="5" t="s">
-        <v>43</v>
-      </c>
-      <c r="U2" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="V2" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="X2" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="Y2" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="Z2" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="AA2" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>51</v>
-      </c>
-      <c r="AC2" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="AD2" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="AE2" s="5" t="s">
-        <v>62</v>
-      </c>
-      <c r="AF2" s="5" t="s">
-        <v>63</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CRM-4377 : Add Inactive SF also in SF Document List Download with Active and Inactive status
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/SF_List_Template.xlsx
+++ b/application/controllers/excel-templates/SF_List_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\XAMPP\htdocs\247_dev\application\controllers\excel-templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dev\application\controllers\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6AB5D775-20E5-4992-A0B6-6C3C03DC0B19}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21A5DA4-FCFF-41C4-AB2E-6777F2D115E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Name</t>
   </si>
@@ -206,6 +206,18 @@
   </si>
   <si>
     <t>{vendor:sf_rm_phone}</t>
+  </si>
+  <si>
+    <t>{vendor:company_name}</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>{vendor:active_status}</t>
+  </si>
+  <si>
+    <t>Company Name</t>
   </si>
 </sst>
 </file>
@@ -577,231 +589,244 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AE2"/>
+  <dimension ref="A1:AG2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="Y1" workbookViewId="0">
-      <selection activeCell="AF1" sqref="AF1:AF1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="37.42578125" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" customWidth="1"/>
-    <col min="3" max="3" width="22" customWidth="1"/>
-    <col min="4" max="5" width="24.140625" customWidth="1"/>
-    <col min="6" max="6" width="19.85546875" customWidth="1"/>
-    <col min="7" max="7" width="18" customWidth="1"/>
-    <col min="8" max="8" width="24.5703125" customWidth="1"/>
-    <col min="9" max="9" width="18.7109375" customWidth="1"/>
-    <col min="10" max="10" width="17.7109375" customWidth="1"/>
-    <col min="11" max="11" width="17.28515625" customWidth="1"/>
-    <col min="12" max="15" width="26.85546875" customWidth="1"/>
-    <col min="16" max="16" width="37.5703125" customWidth="1"/>
-    <col min="17" max="17" width="28" customWidth="1"/>
-    <col min="18" max="18" width="25.5703125" customWidth="1"/>
-    <col min="19" max="19" width="15.5703125" customWidth="1"/>
-    <col min="20" max="20" width="24.5703125" customWidth="1"/>
-    <col min="21" max="21" width="22.28515625" customWidth="1"/>
-    <col min="22" max="22" width="20.42578125" customWidth="1"/>
-    <col min="23" max="23" width="22" customWidth="1"/>
-    <col min="24" max="24" width="25.140625" customWidth="1"/>
-    <col min="25" max="25" width="23.42578125" customWidth="1"/>
-    <col min="26" max="26" width="25.5703125" customWidth="1"/>
-    <col min="27" max="27" width="25.28515625" customWidth="1"/>
-    <col min="28" max="28" width="27.140625" customWidth="1"/>
-    <col min="29" max="29" width="30.140625" customWidth="1"/>
-    <col min="30" max="30" width="22.7109375" customWidth="1"/>
-    <col min="31" max="31" width="27.28515625" customWidth="1"/>
+    <col min="1" max="2" width="37.44140625" customWidth="1"/>
+    <col min="3" max="3" width="36.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22" customWidth="1"/>
+    <col min="5" max="6" width="24.109375" customWidth="1"/>
+    <col min="7" max="7" width="19.88671875" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
+    <col min="9" max="9" width="24.5546875" customWidth="1"/>
+    <col min="10" max="10" width="18.6640625" customWidth="1"/>
+    <col min="11" max="11" width="17.6640625" customWidth="1"/>
+    <col min="12" max="12" width="17.33203125" customWidth="1"/>
+    <col min="13" max="16" width="26.88671875" customWidth="1"/>
+    <col min="17" max="17" width="37.5546875" customWidth="1"/>
+    <col min="18" max="18" width="28" customWidth="1"/>
+    <col min="19" max="19" width="25.5546875" customWidth="1"/>
+    <col min="20" max="20" width="15.5546875" customWidth="1"/>
+    <col min="21" max="21" width="24.5546875" customWidth="1"/>
+    <col min="22" max="22" width="22.33203125" customWidth="1"/>
+    <col min="23" max="23" width="20.44140625" customWidth="1"/>
+    <col min="24" max="24" width="22" customWidth="1"/>
+    <col min="25" max="25" width="25.109375" customWidth="1"/>
+    <col min="26" max="26" width="23.44140625" customWidth="1"/>
+    <col min="27" max="27" width="25.5546875" customWidth="1"/>
+    <col min="28" max="28" width="25.33203125" customWidth="1"/>
+    <col min="29" max="29" width="27.109375" customWidth="1"/>
+    <col min="30" max="30" width="30.109375" customWidth="1"/>
+    <col min="31" max="31" width="22.6640625" customWidth="1"/>
+    <col min="32" max="32" width="33.88671875" customWidth="1"/>
+    <col min="33" max="33" width="21.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AD1" s="4" t="s">
+      <c r="AE1" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>59</v>
       </c>
+      <c r="AG1" s="2" t="s">
+        <v>63</v>
+      </c>
     </row>
-    <row r="2" spans="1:31" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="C2" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="D2" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="E2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="F2" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="5" t="s">
+      <c r="G2" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="G2" s="5" t="s">
+      <c r="H2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="I2" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="J2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="L2" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="M2" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="N2" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="N2" s="5" t="s">
+      <c r="O2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="T2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="U2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="V2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="W2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="X2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="Y2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="Z2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="AA2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>49</v>
       </c>
-      <c r="AB2" s="5" t="s">
+      <c r="AC2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="AC2" s="5" t="s">
+      <c r="AD2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="AD2" s="5" t="s">
+      <c r="AE2" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="AE2" s="5" t="s">
+      <c r="AF2" s="5" t="s">
         <v>61</v>
+      </c>
+      <c r="AG2" s="5" t="s">
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Both ON/OFF vendors in Download SF List
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/SF_List_Template.xlsx
+++ b/application/controllers/excel-templates/SF_List_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dev\application\controllers\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C21A5DA4-FCFF-41C4-AB2E-6777F2D115E0}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AF22B2-8398-4C35-B379-457B454B5E2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
   <si>
     <t>Name</t>
   </si>
@@ -218,6 +218,12 @@
   </si>
   <si>
     <t>Company Name</t>
+  </si>
+  <si>
+    <t>On/Off</t>
+  </si>
+  <si>
+    <t>{vendor:on_off_status}</t>
   </si>
 </sst>
 </file>
@@ -589,10 +595,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AG2"/>
+  <dimension ref="A1:AH2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AI7" sqref="AI7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -625,9 +631,10 @@
     <col min="31" max="31" width="22.6640625" customWidth="1"/>
     <col min="32" max="32" width="33.88671875" customWidth="1"/>
     <col min="33" max="33" width="21.33203125" customWidth="1"/>
+    <col min="34" max="34" width="20.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -727,8 +734,11 @@
       <c r="AG1" s="2" t="s">
         <v>63</v>
       </c>
+      <c r="AH1" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
-    <row r="2" spans="1:33" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>26</v>
       </c>
@@ -827,6 +837,9 @@
       </c>
       <c r="AG2" s="5" t="s">
         <v>64</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CRM-5768 : Show RM and SF name in download sf list
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/SF_List_Template.xlsx
+++ b/application/controllers/excel-templates/SF_List_Template.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dev\application\controllers\excel-templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\temp\application\controllers\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3AF22B2-8398-4C35-B379-457B454B5E2F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1DB298-B2AC-48D0-9994-B337615607BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>Name</t>
   </si>
@@ -196,12 +196,6 @@
     <t>{vendor:gst_status}</t>
   </si>
   <si>
-    <t>Regional Manager Name</t>
-  </si>
-  <si>
-    <t>Regional Manager Contact Name</t>
-  </si>
-  <si>
     <t>{vendor:sf_rm_name}</t>
   </si>
   <si>
@@ -224,6 +218,24 @@
   </si>
   <si>
     <t>{vendor:on_off_status}</t>
+  </si>
+  <si>
+    <t>RM Name</t>
+  </si>
+  <si>
+    <t>RM Contact No</t>
+  </si>
+  <si>
+    <t>ASM Name</t>
+  </si>
+  <si>
+    <t>ASM Contact No</t>
+  </si>
+  <si>
+    <t>{vendor:sf_asm_name}</t>
+  </si>
+  <si>
+    <t>{vendor:sf_asm_phone}</t>
   </si>
 </sst>
 </file>
@@ -595,10 +607,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AH2"/>
+  <dimension ref="A1:AJ2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="AI7" sqref="AI7"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AH8" sqref="AH8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -629,17 +641,17 @@
     <col min="29" max="29" width="27.109375" customWidth="1"/>
     <col min="30" max="30" width="30.109375" customWidth="1"/>
     <col min="31" max="31" width="22.6640625" customWidth="1"/>
-    <col min="32" max="32" width="33.88671875" customWidth="1"/>
-    <col min="33" max="33" width="21.33203125" customWidth="1"/>
-    <col min="34" max="34" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="32" max="34" width="33.88671875" customWidth="1"/>
+    <col min="35" max="35" width="21.33203125" customWidth="1"/>
+    <col min="36" max="36" width="20.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -726,24 +738,30 @@
         <v>25</v>
       </c>
       <c r="AE1" s="4" t="s">
-        <v>58</v>
+        <v>66</v>
       </c>
       <c r="AF1" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="AG1" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="AH1" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
+      </c>
+      <c r="AG1" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="AH1" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:34" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>27</v>
@@ -830,16 +848,22 @@
         <v>51</v>
       </c>
       <c r="AE2" s="5" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="AF2" s="5" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="AG2" s="5" t="s">
-        <v>64</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>67</v>
+        <v>70</v>
+      </c>
+      <c r="AH2" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="AI2" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#CRMS-2119 - PAN number missing in SF details file downloadable from CRM
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/SF_List_Template.xlsx
+++ b/application/controllers/excel-templates/SF_List_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\temp\application\controllers\excel-templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/247around-adminp-aws/application/controllers/excel-templates/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1DB298-B2AC-48D0-9994-B337615607BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7983FD3-28F0-0941-B88D-B927A1267E24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>Name</t>
   </si>
@@ -236,6 +236,12 @@
   </si>
   <si>
     <t>{vendor:sf_asm_phone}</t>
+  </si>
+  <si>
+    <t>PAN</t>
+  </si>
+  <si>
+    <t>{vendor:pan_no}</t>
   </si>
 </sst>
 </file>
@@ -607,46 +613,46 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AJ2"/>
+  <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AH8" sqref="AH8"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="N2" sqref="N2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="37.44140625" customWidth="1"/>
+    <col min="1" max="2" width="37.5" customWidth="1"/>
     <col min="3" max="3" width="36.6640625" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="6" width="24.109375" customWidth="1"/>
-    <col min="7" max="7" width="19.88671875" customWidth="1"/>
+    <col min="5" max="6" width="24.1640625" customWidth="1"/>
+    <col min="7" max="7" width="19.83203125" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="24.5546875" customWidth="1"/>
+    <col min="9" max="9" width="24.5" customWidth="1"/>
     <col min="10" max="10" width="18.6640625" customWidth="1"/>
     <col min="11" max="11" width="17.6640625" customWidth="1"/>
     <col min="12" max="12" width="17.33203125" customWidth="1"/>
-    <col min="13" max="16" width="26.88671875" customWidth="1"/>
-    <col min="17" max="17" width="37.5546875" customWidth="1"/>
-    <col min="18" max="18" width="28" customWidth="1"/>
-    <col min="19" max="19" width="25.5546875" customWidth="1"/>
-    <col min="20" max="20" width="15.5546875" customWidth="1"/>
-    <col min="21" max="21" width="24.5546875" customWidth="1"/>
-    <col min="22" max="22" width="22.33203125" customWidth="1"/>
-    <col min="23" max="23" width="20.44140625" customWidth="1"/>
-    <col min="24" max="24" width="22" customWidth="1"/>
-    <col min="25" max="25" width="25.109375" customWidth="1"/>
-    <col min="26" max="26" width="23.44140625" customWidth="1"/>
-    <col min="27" max="27" width="25.5546875" customWidth="1"/>
-    <col min="28" max="28" width="25.33203125" customWidth="1"/>
-    <col min="29" max="29" width="27.109375" customWidth="1"/>
-    <col min="30" max="30" width="30.109375" customWidth="1"/>
-    <col min="31" max="31" width="22.6640625" customWidth="1"/>
-    <col min="32" max="34" width="33.88671875" customWidth="1"/>
-    <col min="35" max="35" width="21.33203125" customWidth="1"/>
-    <col min="36" max="36" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="17" width="26.83203125" customWidth="1"/>
+    <col min="18" max="18" width="37.5" customWidth="1"/>
+    <col min="19" max="19" width="28" customWidth="1"/>
+    <col min="20" max="20" width="25.5" customWidth="1"/>
+    <col min="21" max="21" width="15.5" customWidth="1"/>
+    <col min="22" max="22" width="24.5" customWidth="1"/>
+    <col min="23" max="23" width="22.33203125" customWidth="1"/>
+    <col min="24" max="24" width="20.5" customWidth="1"/>
+    <col min="25" max="25" width="22" customWidth="1"/>
+    <col min="26" max="26" width="25.1640625" customWidth="1"/>
+    <col min="27" max="27" width="23.5" customWidth="1"/>
+    <col min="28" max="28" width="25.5" customWidth="1"/>
+    <col min="29" max="29" width="25.33203125" customWidth="1"/>
+    <col min="30" max="30" width="27.1640625" customWidth="1"/>
+    <col min="31" max="31" width="30.1640625" customWidth="1"/>
+    <col min="32" max="32" width="22.6640625" customWidth="1"/>
+    <col min="33" max="35" width="33.83203125" customWidth="1"/>
+    <col min="36" max="36" width="21.33203125" customWidth="1"/>
+    <col min="37" max="37" width="20.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -687,76 +693,79 @@
         <v>11</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="5" t="s">
         <v>26</v>
       </c>
@@ -797,72 +806,75 @@
         <v>37</v>
       </c>
       <c r="N2" s="5" t="s">
+        <v>73</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="T2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="U2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="V2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="W2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="X2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="Y2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="Z2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="AA2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AB2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>49</v>
       </c>
-      <c r="AC2" s="5" t="s">
+      <c r="AD2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="AD2" s="5" t="s">
+      <c r="AE2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="AE2" s="5" t="s">
+      <c r="AF2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AF2" s="5" t="s">
+      <c r="AG2" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="AG2" s="5" t="s">
+      <c r="AH2" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="AH2" s="5" t="s">
+      <c r="AI2" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AI2" s="5" t="s">
+      <c r="AJ2" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CRMS-2314 Enter PAN number column
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/SF_List_Template.xlsx
+++ b/application/controllers/excel-templates/SF_List_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\temp\application\controllers\excel-templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\release\application\controllers\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F1DB298-B2AC-48D0-9994-B337615607BB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62344EF6-A4ED-4586-ADDF-AFD4D3193EFC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>Name</t>
   </si>
@@ -236,6 +236,12 @@
   </si>
   <si>
     <t>{vendor:sf_asm_phone}</t>
+  </si>
+  <si>
+    <t>{vendor:pan_no}</t>
+  </si>
+  <si>
+    <t>PAN</t>
   </si>
 </sst>
 </file>
@@ -607,46 +613,46 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AJ2"/>
+  <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
-      <selection activeCell="AH8" sqref="AH8"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="O1" sqref="O1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="37.44140625" customWidth="1"/>
-    <col min="3" max="3" width="36.6640625" customWidth="1"/>
+    <col min="1" max="2" width="37.42578125" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="6" width="24.109375" customWidth="1"/>
-    <col min="7" max="7" width="19.88671875" customWidth="1"/>
+    <col min="5" max="6" width="24.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="24.5546875" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" customWidth="1"/>
-    <col min="12" max="12" width="17.33203125" customWidth="1"/>
-    <col min="13" max="16" width="26.88671875" customWidth="1"/>
-    <col min="17" max="17" width="37.5546875" customWidth="1"/>
-    <col min="18" max="18" width="28" customWidth="1"/>
-    <col min="19" max="19" width="25.5546875" customWidth="1"/>
-    <col min="20" max="20" width="15.5546875" customWidth="1"/>
-    <col min="21" max="21" width="24.5546875" customWidth="1"/>
-    <col min="22" max="22" width="22.33203125" customWidth="1"/>
-    <col min="23" max="23" width="20.44140625" customWidth="1"/>
-    <col min="24" max="24" width="22" customWidth="1"/>
-    <col min="25" max="25" width="25.109375" customWidth="1"/>
-    <col min="26" max="26" width="23.44140625" customWidth="1"/>
-    <col min="27" max="27" width="25.5546875" customWidth="1"/>
-    <col min="28" max="28" width="25.33203125" customWidth="1"/>
-    <col min="29" max="29" width="27.109375" customWidth="1"/>
-    <col min="30" max="30" width="30.109375" customWidth="1"/>
-    <col min="31" max="31" width="22.6640625" customWidth="1"/>
-    <col min="32" max="34" width="33.88671875" customWidth="1"/>
-    <col min="35" max="35" width="21.33203125" customWidth="1"/>
-    <col min="36" max="36" width="20.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.5703125" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" customWidth="1"/>
+    <col min="13" max="17" width="26.85546875" customWidth="1"/>
+    <col min="18" max="18" width="37.5703125" customWidth="1"/>
+    <col min="19" max="19" width="28" customWidth="1"/>
+    <col min="20" max="20" width="25.5703125" customWidth="1"/>
+    <col min="21" max="21" width="15.5703125" customWidth="1"/>
+    <col min="22" max="22" width="24.5703125" customWidth="1"/>
+    <col min="23" max="23" width="22.28515625" customWidth="1"/>
+    <col min="24" max="24" width="20.42578125" customWidth="1"/>
+    <col min="25" max="25" width="22" customWidth="1"/>
+    <col min="26" max="26" width="25.140625" customWidth="1"/>
+    <col min="27" max="27" width="23.42578125" customWidth="1"/>
+    <col min="28" max="28" width="25.5703125" customWidth="1"/>
+    <col min="29" max="29" width="25.28515625" customWidth="1"/>
+    <col min="30" max="30" width="27.140625" customWidth="1"/>
+    <col min="31" max="31" width="30.140625" customWidth="1"/>
+    <col min="32" max="32" width="22.7109375" customWidth="1"/>
+    <col min="33" max="35" width="33.85546875" customWidth="1"/>
+    <col min="36" max="36" width="21.28515625" customWidth="1"/>
+    <col min="37" max="37" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -687,76 +693,79 @@
         <v>11</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="AI1" s="2" t="s">
+      <c r="AJ1" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="2" spans="1:36" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>26</v>
       </c>
@@ -797,72 +806,75 @@
         <v>37</v>
       </c>
       <c r="N2" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="P2" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="Q2" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="T2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="U2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="V2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="W2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="X2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="Y2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="Z2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="AA2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AB2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>49</v>
       </c>
-      <c r="AC2" s="5" t="s">
+      <c r="AD2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="AD2" s="5" t="s">
+      <c r="AE2" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="AE2" s="5" t="s">
+      <c r="AF2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AF2" s="5" t="s">
+      <c r="AG2" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="AG2" s="5" t="s">
+      <c r="AH2" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="AH2" s="5" t="s">
+      <c r="AI2" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AI2" s="5" t="s">
+      <c r="AJ2" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>65</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CRMS-2226 Add MSME Number Column in SF Download List
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/SF_List_Template.xlsx
+++ b/application/controllers/excel-templates/SF_List_Template.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
-  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\release\application\controllers\excel-templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\integration\application\controllers\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D325ECA-6DC7-4A83-B53A-5D11168084F7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="76">
   <si>
     <t>Name</t>
   </si>
@@ -242,12 +241,18 @@
   </si>
   <si>
     <t>{vendor:sf_create_date}</t>
+  </si>
+  <si>
+    <t>MSME Number</t>
+  </si>
+  <si>
+    <t>{vendor:msme_no}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -611,48 +616,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AK2"/>
+  <dimension ref="A1:AL2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="X1" workbookViewId="0">
-      <selection activeCell="AC2" sqref="AC2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="2" width="37.42578125" customWidth="1"/>
-    <col min="3" max="3" width="36.7109375" customWidth="1"/>
+    <col min="1" max="2" width="37.453125" customWidth="1"/>
+    <col min="3" max="3" width="36.7265625" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="6" width="24.140625" customWidth="1"/>
-    <col min="7" max="7" width="19.85546875" customWidth="1"/>
+    <col min="5" max="6" width="24.1796875" customWidth="1"/>
+    <col min="7" max="7" width="19.81640625" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="24.5703125" customWidth="1"/>
-    <col min="10" max="10" width="18.7109375" customWidth="1"/>
-    <col min="11" max="11" width="17.7109375" customWidth="1"/>
-    <col min="12" max="12" width="17.28515625" customWidth="1"/>
-    <col min="13" max="17" width="26.85546875" customWidth="1"/>
-    <col min="18" max="18" width="37.5703125" customWidth="1"/>
+    <col min="9" max="9" width="24.54296875" customWidth="1"/>
+    <col min="10" max="10" width="18.7265625" customWidth="1"/>
+    <col min="11" max="11" width="17.7265625" customWidth="1"/>
+    <col min="12" max="12" width="17.26953125" customWidth="1"/>
+    <col min="13" max="17" width="26.81640625" customWidth="1"/>
+    <col min="18" max="18" width="37.54296875" customWidth="1"/>
     <col min="19" max="19" width="28" customWidth="1"/>
-    <col min="20" max="20" width="25.5703125" customWidth="1"/>
-    <col min="21" max="21" width="15.5703125" customWidth="1"/>
-    <col min="22" max="22" width="24.5703125" customWidth="1"/>
-    <col min="23" max="23" width="22.28515625" customWidth="1"/>
-    <col min="24" max="24" width="20.42578125" customWidth="1"/>
+    <col min="20" max="20" width="25.54296875" customWidth="1"/>
+    <col min="21" max="21" width="15.54296875" customWidth="1"/>
+    <col min="22" max="22" width="24.54296875" customWidth="1"/>
+    <col min="23" max="23" width="22.26953125" customWidth="1"/>
+    <col min="24" max="24" width="20.453125" customWidth="1"/>
     <col min="25" max="25" width="22" customWidth="1"/>
-    <col min="26" max="26" width="25.140625" customWidth="1"/>
-    <col min="27" max="27" width="23.42578125" customWidth="1"/>
-    <col min="28" max="28" width="25.5703125" customWidth="1"/>
-    <col min="29" max="29" width="25.28515625" customWidth="1"/>
-    <col min="30" max="30" width="27.140625" customWidth="1"/>
-    <col min="31" max="31" width="30.140625" customWidth="1"/>
-    <col min="32" max="32" width="22.7109375" customWidth="1"/>
-    <col min="33" max="35" width="33.85546875" customWidth="1"/>
-    <col min="36" max="36" width="21.28515625" customWidth="1"/>
-    <col min="37" max="37" width="20.28515625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="25.1796875" customWidth="1"/>
+    <col min="27" max="27" width="23.453125" customWidth="1"/>
+    <col min="28" max="28" width="25.54296875" customWidth="1"/>
+    <col min="29" max="29" width="25.26953125" customWidth="1"/>
+    <col min="30" max="30" width="27.1796875" customWidth="1"/>
+    <col min="31" max="31" width="30.1796875" customWidth="1"/>
+    <col min="32" max="32" width="22.7265625" customWidth="1"/>
+    <col min="33" max="35" width="33.81640625" customWidth="1"/>
+    <col min="36" max="36" width="21.26953125" customWidth="1"/>
+    <col min="37" max="37" width="20.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -699,73 +704,76 @@
         <v>51</v>
       </c>
       <c r="P1" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="AI1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="AJ1" s="2" t="s">
+      <c r="AK1" s="2" t="s">
         <v>60</v>
       </c>
-      <c r="AK1" s="2" t="s">
+      <c r="AL1" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>26</v>
       </c>
@@ -812,69 +820,72 @@
         <v>52</v>
       </c>
       <c r="P2" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="Q2" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="R2" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="S2" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="T2" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="U2" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="V2" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="V2" s="5" t="s">
+      <c r="W2" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="X2" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="X2" s="5" t="s">
+      <c r="Y2" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="Z2" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="AA2" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AB2" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="AB2" s="5" t="s">
+      <c r="AC2" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>73</v>
       </c>
-      <c r="AD2" s="5" t="s">
+      <c r="AE2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="AE2" s="5" t="s">
+      <c r="AF2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="AF2" s="5" t="s">
+      <c r="AG2" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="AG2" s="5" t="s">
+      <c r="AH2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AH2" s="5" t="s">
+      <c r="AI2" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="AI2" s="5" t="s">
+      <c r="AJ2" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="AJ2" s="5" t="s">
+      <c r="AK2" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="AK2" t="s">
+      <c r="AL2" t="s">
         <v>64</v>
       </c>
     </row>

</xml_diff>

<commit_message>
CRMS-2226 add MSME number column
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/SF_List_Template.xlsx
+++ b/application/controllers/excel-templates/SF_List_Template.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Applications/MAMP/htdocs/247around-adminp-aws/application/controllers/excel-templates/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dev\application\controllers\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7983FD3-28F0-0941-B88D-B927A1267E24}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53910DD-48FE-4CB4-B256-A5D62ECD124D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>Name</t>
   </si>
@@ -187,9 +187,6 @@
     <t>GST Type</t>
   </si>
   <si>
-    <t>{vendor:gst_taxpayer_type}</t>
-  </si>
-  <si>
     <t>GST Status</t>
   </si>
   <si>
@@ -238,10 +235,16 @@
     <t>{vendor:sf_asm_phone}</t>
   </si>
   <si>
-    <t>PAN</t>
-  </si>
-  <si>
     <t>{vendor:pan_no}</t>
+  </si>
+  <si>
+    <t>MSME Number</t>
+  </si>
+  <si>
+    <t>PAN Number</t>
+  </si>
+  <si>
+    <t>{vendor:msme_no}</t>
   </si>
 </sst>
 </file>
@@ -613,51 +616,51 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AK2"/>
+  <dimension ref="A1:AL2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="P2" sqref="P2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="37.5" customWidth="1"/>
-    <col min="3" max="3" width="36.6640625" customWidth="1"/>
+    <col min="1" max="2" width="37.42578125" customWidth="1"/>
+    <col min="3" max="3" width="36.7109375" customWidth="1"/>
     <col min="4" max="4" width="22" customWidth="1"/>
-    <col min="5" max="6" width="24.1640625" customWidth="1"/>
-    <col min="7" max="7" width="19.83203125" customWidth="1"/>
+    <col min="5" max="6" width="24.140625" customWidth="1"/>
+    <col min="7" max="7" width="19.85546875" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="24.5" customWidth="1"/>
-    <col min="10" max="10" width="18.6640625" customWidth="1"/>
-    <col min="11" max="11" width="17.6640625" customWidth="1"/>
-    <col min="12" max="12" width="17.33203125" customWidth="1"/>
-    <col min="13" max="17" width="26.83203125" customWidth="1"/>
-    <col min="18" max="18" width="37.5" customWidth="1"/>
+    <col min="9" max="9" width="24.42578125" customWidth="1"/>
+    <col min="10" max="10" width="18.7109375" customWidth="1"/>
+    <col min="11" max="11" width="17.7109375" customWidth="1"/>
+    <col min="12" max="12" width="17.28515625" customWidth="1"/>
+    <col min="13" max="17" width="26.85546875" customWidth="1"/>
+    <col min="18" max="18" width="37.42578125" customWidth="1"/>
     <col min="19" max="19" width="28" customWidth="1"/>
-    <col min="20" max="20" width="25.5" customWidth="1"/>
-    <col min="21" max="21" width="15.5" customWidth="1"/>
-    <col min="22" max="22" width="24.5" customWidth="1"/>
-    <col min="23" max="23" width="22.33203125" customWidth="1"/>
-    <col min="24" max="24" width="20.5" customWidth="1"/>
+    <col min="20" max="20" width="25.42578125" customWidth="1"/>
+    <col min="21" max="21" width="15.42578125" customWidth="1"/>
+    <col min="22" max="22" width="24.42578125" customWidth="1"/>
+    <col min="23" max="23" width="22.28515625" customWidth="1"/>
+    <col min="24" max="24" width="20.42578125" customWidth="1"/>
     <col min="25" max="25" width="22" customWidth="1"/>
-    <col min="26" max="26" width="25.1640625" customWidth="1"/>
-    <col min="27" max="27" width="23.5" customWidth="1"/>
-    <col min="28" max="28" width="25.5" customWidth="1"/>
-    <col min="29" max="29" width="25.33203125" customWidth="1"/>
-    <col min="30" max="30" width="27.1640625" customWidth="1"/>
-    <col min="31" max="31" width="30.1640625" customWidth="1"/>
-    <col min="32" max="32" width="22.6640625" customWidth="1"/>
-    <col min="33" max="35" width="33.83203125" customWidth="1"/>
-    <col min="36" max="36" width="21.33203125" customWidth="1"/>
-    <col min="37" max="37" width="20.1640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="25.140625" customWidth="1"/>
+    <col min="27" max="27" width="23.42578125" customWidth="1"/>
+    <col min="28" max="28" width="25.42578125" customWidth="1"/>
+    <col min="29" max="29" width="25.28515625" customWidth="1"/>
+    <col min="30" max="30" width="27.140625" customWidth="1"/>
+    <col min="31" max="31" width="30.140625" customWidth="1"/>
+    <col min="32" max="32" width="22.7109375" customWidth="1"/>
+    <col min="33" max="35" width="33.85546875" customWidth="1"/>
+    <col min="36" max="36" width="21.28515625" customWidth="1"/>
+    <col min="37" max="37" width="20.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -693,84 +696,87 @@
         <v>11</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>52</v>
       </c>
       <c r="P1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q1" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="R1" s="1" t="s">
+      <c r="R1" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AA1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AB1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AC1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AD1" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AE1" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="AE1" s="1" t="s">
+      <c r="AF1" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AJ1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="AI1" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>61</v>
-      </c>
       <c r="AK1" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>27</v>
@@ -806,16 +812,16 @@
         <v>37</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="O2" s="5" t="s">
         <v>53</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>38</v>
@@ -860,22 +866,22 @@
         <v>51</v>
       </c>
       <c r="AF2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AG2" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="AH2" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI2" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="AI2" s="5" t="s">
-        <v>71</v>
-      </c>
       <c r="AJ2" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AK2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CRMS-2395 Update Create date column in excel
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/SF_List_Template.xlsx
+++ b/application/controllers/excel-templates/SF_List_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\release\application\controllers\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62344EF6-A4ED-4586-ADDF-AFD4D3193EFC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5F2503-E361-4663-B8C4-23CFA9F44E36}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -169,9 +169,6 @@
     <t>{vendor:owner_phone_2}</t>
   </si>
   <si>
-    <t>{vendor:create_date}</t>
-  </si>
-  <si>
     <t>{vendor:non_working_days}</t>
   </si>
   <si>
@@ -242,6 +239,9 @@
   </si>
   <si>
     <t>PAN</t>
+  </si>
+  <si>
+    <t>{vendor:sf_create_date</t>
   </si>
 </sst>
 </file>
@@ -615,8 +615,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="O1" sqref="O1"/>
+    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -657,7 +657,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
@@ -693,16 +693,16 @@
         <v>11</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R1" s="1" t="s">
         <v>12</v>
@@ -747,22 +747,22 @@
         <v>25</v>
       </c>
       <c r="AF1" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="AG1" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AH1" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="AH1" s="4" t="s">
+      <c r="AI1" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="AI1" s="4" t="s">
-        <v>69</v>
-      </c>
       <c r="AJ1" s="2" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AK1" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -770,7 +770,7 @@
         <v>26</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>27</v>
@@ -806,16 +806,16 @@
         <v>37</v>
       </c>
       <c r="N2" s="5" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="Q2" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="R2" s="5" t="s">
         <v>38</v>
@@ -851,31 +851,31 @@
         <v>48</v>
       </c>
       <c r="AC2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="AD2" s="5" t="s">
+      <c r="AE2" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="AE2" s="5" t="s">
-        <v>51</v>
-      </c>
       <c r="AF2" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="AG2" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="AG2" s="5" t="s">
-        <v>59</v>
-      </c>
       <c r="AH2" s="5" t="s">
+        <v>69</v>
+      </c>
+      <c r="AI2" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="AI2" s="5" t="s">
-        <v>71</v>
-      </c>
       <c r="AJ2" s="5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="AK2" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CRMS-2395 correct create date
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/SF_List_Template.xlsx
+++ b/application/controllers/excel-templates/SF_List_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\dev\application\controllers\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C53910DD-48FE-4CB4-B256-A5D62ECD124D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7703DB5C-4627-4231-A60E-B3BAA68C859D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>Name</t>
   </si>
@@ -169,9 +169,6 @@
     <t>{vendor:owner_phone_2}</t>
   </si>
   <si>
-    <t>{vendor:create_date}</t>
-  </si>
-  <si>
     <t>{vendor:non_working_days}</t>
   </si>
   <si>
@@ -187,6 +184,9 @@
     <t>GST Type</t>
   </si>
   <si>
+    <t>{vendor:gst_taxpayer_type}</t>
+  </si>
+  <si>
     <t>GST Status</t>
   </si>
   <si>
@@ -238,13 +238,10 @@
     <t>{vendor:pan_no}</t>
   </si>
   <si>
-    <t>MSME Number</t>
-  </si>
-  <si>
-    <t>PAN Number</t>
-  </si>
-  <si>
-    <t>{vendor:msme_no}</t>
+    <t>PAN</t>
+  </si>
+  <si>
+    <t>{vendor:sf_create_date}</t>
   </si>
 </sst>
 </file>
@@ -616,10 +613,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1"/>
-  <dimension ref="A1:AL2"/>
+  <dimension ref="A1:AK2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AC2" sqref="AC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -630,32 +627,32 @@
     <col min="5" max="6" width="24.140625" customWidth="1"/>
     <col min="7" max="7" width="19.85546875" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="24.42578125" customWidth="1"/>
+    <col min="9" max="9" width="24.5703125" customWidth="1"/>
     <col min="10" max="10" width="18.7109375" customWidth="1"/>
     <col min="11" max="11" width="17.7109375" customWidth="1"/>
     <col min="12" max="12" width="17.28515625" customWidth="1"/>
     <col min="13" max="17" width="26.85546875" customWidth="1"/>
-    <col min="18" max="18" width="37.42578125" customWidth="1"/>
+    <col min="18" max="18" width="37.5703125" customWidth="1"/>
     <col min="19" max="19" width="28" customWidth="1"/>
-    <col min="20" max="20" width="25.42578125" customWidth="1"/>
-    <col min="21" max="21" width="15.42578125" customWidth="1"/>
-    <col min="22" max="22" width="24.42578125" customWidth="1"/>
+    <col min="20" max="20" width="25.5703125" customWidth="1"/>
+    <col min="21" max="21" width="15.5703125" customWidth="1"/>
+    <col min="22" max="22" width="24.5703125" customWidth="1"/>
     <col min="23" max="23" width="22.28515625" customWidth="1"/>
     <col min="24" max="24" width="20.42578125" customWidth="1"/>
     <col min="25" max="25" width="22" customWidth="1"/>
     <col min="26" max="26" width="25.140625" customWidth="1"/>
     <col min="27" max="27" width="23.42578125" customWidth="1"/>
-    <col min="28" max="28" width="25.42578125" customWidth="1"/>
+    <col min="28" max="28" width="25.5703125" customWidth="1"/>
     <col min="29" max="29" width="25.28515625" customWidth="1"/>
     <col min="30" max="30" width="27.140625" customWidth="1"/>
     <col min="31" max="31" width="30.140625" customWidth="1"/>
     <col min="32" max="32" width="22.7109375" customWidth="1"/>
     <col min="33" max="35" width="33.85546875" customWidth="1"/>
     <col min="36" max="36" width="21.28515625" customWidth="1"/>
-    <col min="37" max="37" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="20.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -696,82 +693,79 @@
         <v>11</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>72</v>
+        <v>53</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="R1" s="2" t="s">
         <v>55</v>
       </c>
+      <c r="R1" s="1" t="s">
+        <v>12</v>
+      </c>
       <c r="S1" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="Z1" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AA1" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AB1" s="1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AC1" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AD1" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AE1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AF1" s="1" t="s">
         <v>25</v>
       </c>
+      <c r="AF1" s="4" t="s">
+        <v>65</v>
+      </c>
       <c r="AG1" s="4" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="AH1" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="AI1" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="AJ1" s="4" t="s">
         <v>68</v>
       </c>
+      <c r="AJ1" s="2" t="s">
+        <v>60</v>
+      </c>
       <c r="AK1" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="AL1" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="2" spans="1:38" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:37" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
         <v>26</v>
       </c>
@@ -815,10 +809,10 @@
         <v>71</v>
       </c>
       <c r="O2" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="P2" s="5" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="Q2" s="5" t="s">
         <v>56</v>
@@ -857,13 +851,13 @@
         <v>48</v>
       </c>
       <c r="AC2" t="s">
+        <v>73</v>
+      </c>
+      <c r="AD2" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="AD2" s="5" t="s">
+      <c r="AE2" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="AE2" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="AF2" s="5" t="s">
         <v>57</v>

</xml_diff>

<commit_message>
CRMS-2395 update in excel
</commit_message>
<xml_diff>
--- a/application/controllers/excel-templates/SF_List_Template.xlsx
+++ b/application/controllers/excel-templates/SF_List_Template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\release\application\controllers\excel-templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E5F2503-E361-4663-B8C4-23CFA9F44E36}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78397E36-74FD-4305-8F5A-B12DE514561A}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -241,7 +241,7 @@
     <t>PAN</t>
   </si>
   <si>
-    <t>{vendor:sf_create_date</t>
+    <t>{vendor:sf_create_date}</t>
   </si>
 </sst>
 </file>

</xml_diff>